<commit_message>
update to interpolation methodology
</commit_message>
<xml_diff>
--- a/Travis_County/Documentation/Travis_County_2018_bg_config.xlsx
+++ b/Travis_County/Documentation/Travis_County_2018_bg_config.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,67 +452,84 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>F1: 1</t>
+          <t>F2: 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F1: 1</t>
+          <t>F2: 1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['QSERV' 'PPUNIT' 'QEDLESHI' 'QESL' 'QEXTRCT' 'QHISPC' 'QNOHLTH' 'PERCAP'
- 'QFHH']</t>
+          <t>['QNOHLTH' 'QHISPC' 'PPUNIT' 'QSERV' 'QESL' 'QEDLESHI' 'QEXTRCT' 'QFHH'
+ 'PERCAP']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>F1: 2</t>
+          <t>F2: 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F1: 2</t>
+          <t>F2: 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['QNOHLTH' 'QRICH' 'PERCAP' 'QRENTER' 'QPOVTY' 'QNOAUTO' 'QFAM']</t>
+          <t>['QRICH' 'MDHSEVAL' 'PERCAP']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>F1: 3</t>
+          <t>F2: 3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F1: 3</t>
+          <t>F2: 3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['QAGEDEP' 'MEDAGE' 'QSSBEN']</t>
+          <t>['QRENTER' 'QNOAUTO' 'QPOVTY']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>F1: 4</t>
+          <t>F2: 4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F1: 4</t>
+          <t>F2: 4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t>['MEDAGE' 'QSSBEN' 'QAGEDEP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>F2: 5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>F2: 5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>['QAGEDEP' 'QFEMLBR' 'QFEMALE']</t>
         </is>
@@ -529,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,232 +557,270 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>F1: 1</t>
+          <t>F2: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>F1: 2</t>
+          <t>F2: 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>F1: 3</t>
+          <t>F2: 3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F1: 4</t>
+          <t>F2: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 5</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5819296581136502</v>
+        <v>0.6641941122002464</v>
       </c>
       <c r="C2" t="n">
-        <v>0.419440430948276</v>
+        <v>0.4111007544969877</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1205750347425241</v>
+        <v>0.327159092345672</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.09979277314440696</v>
+        <v>-0.08880591641510853</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.1206077732995754</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7466083339789722</v>
+        <v>0.8172800708240761</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3808868059793599</v>
+        <v>0.3568107832167007</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1350498374295295</v>
+        <v>0.1430522455328176</v>
       </c>
       <c r="E3" t="n">
-        <v>0.07955222377131646</v>
+        <v>-0.1035311703573437</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.1284245812002146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QEDLESHI</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8719904904522056</v>
+        <v>0.7213533591425673</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2240118533062473</v>
+        <v>0.03768695314523186</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0004224679597168181</v>
+        <v>-0.340714441132671</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1268112752795882</v>
+        <v>-0.09293314900396191</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.07082527372821094</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>QESL</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7762414529782653</v>
+        <v>0.517056355052926</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2191701896264946</v>
+        <v>0.3832057679581961</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01086754774744363</v>
+        <v>0.311558311947261</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2337348448502218</v>
+        <v>-0.1307287334302756</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.1013539558858636</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QESL</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7696209836666792</v>
+        <v>0.7916387764699077</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08863346446473094</v>
+        <v>0.1578130985349176</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.008687124693828202</v>
+        <v>0.2139992488008075</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.2324818449561593</v>
+        <v>-0.0314487937301029</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.2060743019298396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>QEDLESHI</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8709706297376701</v>
+        <v>0.8729342608933685</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2440344048993926</v>
+        <v>0.2064110063017868</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.09445653687716601</v>
+        <v>0.2004013888253722</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1311656402055592</v>
+        <v>-0.01618995688075913</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.1067088317849588</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7289577757146266</v>
+        <v>0.7830485250109201</v>
       </c>
       <c r="C8" t="n">
-        <v>0.450258889881075</v>
+        <v>0.1226948168972316</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.06769369393477219</v>
+        <v>0.09276530213712816</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1223822633335377</v>
+        <v>-0.01971134291552629</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.2082444669752325</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>QRICH</t>
+          <t>QFHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4100945798092822</v>
+        <v>0.5607864131566372</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6045963057023201</v>
+        <v>0.2738331457858463</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1952906069957424</v>
+        <v>0.05550829987809005</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0120395063322554</v>
+        <v>-0.06567204376371692</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.2456792748662655</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>PERCAP</t>
+          <t>QRICH</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6228719555521134</v>
+        <v>0.2058450521114599</v>
       </c>
       <c r="C10" t="n">
-        <v>0.493788397409561</v>
+        <v>0.8483747168011316</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.2256556857205278</v>
+        <v>0.3541943659819356</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06576072222188216</v>
+        <v>-0.1749190839245255</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.02690806984672741</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>QAGEDEP</t>
+          <t>MDHSEVAL</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.04452179183186798</v>
+        <v>0.3746877273915546</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1845441741485256</v>
+        <v>0.680310731367022</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7050230831784325</v>
+        <v>-0.1250235556616157</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5788611384463409</v>
+        <v>0.00295119629720828</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.01357761256245511</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>MEDAGE</t>
+          <t>PERCAP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.3376734884122854</v>
+        <v>0.472078660569859</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.4360158142799522</v>
+        <v>0.7110281175952148</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7300625491827496</v>
+        <v>0.2599191305489495</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.02997720941225419</v>
+        <v>-0.2188984120719565</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.04385980555370568</v>
       </c>
     </row>
     <row r="13">
@@ -775,35 +830,41 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.02071031116731996</v>
+        <v>-0.0169865811594124</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7905516668985624</v>
+        <v>0.1782040321943912</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.364473661435097</v>
+        <v>0.7623798549014968</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1374053827757201</v>
+        <v>-0.4175899392239148</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.1129122996727554</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>QSSBEN</t>
+          <t>QNOAUTO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01608283330069052</v>
+        <v>0.1056780863584004</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.2036133255093752</v>
+        <v>0.05350761822061592</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8009829894647723</v>
+        <v>0.6975393916527455</v>
       </c>
       <c r="E14" t="n">
-        <v>0.09085651365625987</v>
+        <v>-0.04914871524614545</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.003119068169388665</v>
       </c>
     </row>
     <row r="15">
@@ -813,111 +874,129 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.293191408326295</v>
+        <v>0.2992888396138256</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5450332184513632</v>
+        <v>0.148607011408278</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.2505318228265868</v>
+        <v>0.5737043965764143</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06302684933295673</v>
+        <v>-0.2807685012847285</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.09516280552966946</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>QNOAUTO</t>
+          <t>MEDAGE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07928337856296344</v>
+        <v>-0.3193244214567408</v>
       </c>
       <c r="C16" t="n">
-        <v>0.615093322921848</v>
+        <v>-0.2200222480200467</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02644631102323169</v>
+        <v>-0.3643133272133273</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.02316762006401123</v>
+        <v>0.7585327102945554</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.04004000901821723</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>QFEMLBR</t>
+          <t>QSSBEN</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.2303346464407058</v>
+        <v>0.005424293531374609</v>
       </c>
       <c r="C17" t="n">
-        <v>0.06590913164096851</v>
+        <v>-0.02898540048679379</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.04164890497918423</v>
+        <v>-0.1541266274192051</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7646973503389133</v>
+        <v>0.829857786771077</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.08691606186838186</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>QFEMALE</t>
+          <t>QAGEDEP</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.03632045086136099</v>
+        <v>-0.01574198855808457</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.02692143941774866</v>
+        <v>-0.1414286087818206</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2164151898146264</v>
+        <v>-0.1080367958173994</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8115652981688578</v>
+        <v>0.6951599658178635</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.5982193179122143</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>QFHH</t>
+          <t>QFEMLBR</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.6171428203259905</v>
+        <v>-0.2609508547515848</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1927279759144678</v>
+        <v>0.07812259117665589</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.0565575333007507</v>
+        <v>2.961441042594403e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2833386145888123</v>
+        <v>-0.04558978074484524</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.7376544298789692</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>QFAM</t>
+          <t>QFEMALE</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2956877377183108</v>
+        <v>-0.01186351313103661</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5130508708856372</v>
+        <v>-0.0748927632368649</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1579596935159818</v>
+        <v>0.008529709894781311</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1055369714480047</v>
+        <v>0.1928293016857023</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.868720233107825</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +1010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,6 +1074,36 @@
           <t>F1: 4</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>F1: 5</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 2</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 3</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 4</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 5</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1003,37 +1112,55 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.69876472017816</v>
+        <v>4.931282064630651</v>
       </c>
       <c r="C2" t="n">
-        <v>2.874191229720769</v>
+        <v>2.797028014906584</v>
       </c>
       <c r="D2" t="n">
-        <v>2.468235508583059</v>
+        <v>2.452495185487878</v>
       </c>
       <c r="E2" t="n">
-        <v>1.941378780384548</v>
+        <v>2.338350485850176</v>
       </c>
       <c r="F2" t="n">
-        <v>1.921579152225509</v>
+        <v>1.91555137023628</v>
       </c>
       <c r="G2" t="n">
-        <v>1.256784679853808</v>
+        <v>1.357471911060389</v>
       </c>
       <c r="H2" t="n">
-        <v>1.232272042224185</v>
+        <v>1.235122303123883</v>
       </c>
       <c r="I2" t="n">
-        <v>5.429027041354204</v>
+        <v>4.626008835319829</v>
       </c>
       <c r="J2" t="n">
-        <v>3.170159058870136</v>
+        <v>3.164090131524766</v>
       </c>
       <c r="K2" t="n">
-        <v>2.08018338849591</v>
+        <v>2.337676532711858</v>
       </c>
       <c r="L2" t="n">
-        <v>1.880141517197375</v>
+        <v>2.168885487825472</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.890316422487597</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.890284008387104</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2.42792500097139</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.212082293812811</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2.170978841433984</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1.894385220306634</v>
       </c>
     </row>
     <row r="3">
@@ -1043,37 +1170,55 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1740283229695615</v>
+        <v>0.1826400764678019</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1064515270266951</v>
+        <v>0.1035936301817253</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0914161299475207</v>
+        <v>0.09083315501806954</v>
       </c>
       <c r="E3" t="n">
-        <v>0.07190291779202031</v>
+        <v>0.08660557355000652</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07116959823057442</v>
+        <v>0.07094634704578816</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04654758073532622</v>
+        <v>0.05027673744668107</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0456397052675624</v>
+        <v>0.04574527048606975</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2857382653344318</v>
+        <v>0.22028613501523</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1668504767826388</v>
+        <v>0.1506709586440365</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1094833362366268</v>
+        <v>0.1113179301291361</v>
       </c>
       <c r="L3" t="n">
-        <v>0.09895481669459867</v>
+        <v>0.1032802613250225</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.09001506773750462</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.2573833688624791</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.1277855263669153</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.1164253838848848</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.1142620442859991</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.0997044852792965</v>
       </c>
     </row>
     <row r="4">
@@ -1083,37 +1228,55 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1740283229695615</v>
+        <v>0.1826400764678019</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2804798499962566</v>
+        <v>0.2862337066495272</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3718959799437773</v>
+        <v>0.3770668616675967</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4437988977357976</v>
+        <v>0.4636724352176033</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5149684959663721</v>
+        <v>0.5346187822633914</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5615160767016982</v>
+        <v>0.5848955197100725</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6071557819692607</v>
+        <v>0.6306407901961423</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2857382653344318</v>
+        <v>0.22028613501523</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4525887421170706</v>
+        <v>0.3709570936592664</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5620720783536974</v>
+        <v>0.4822750237884025</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6610268950482961</v>
+        <v>0.585555285113425</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.6755703528509296</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2573833688624791</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.3851688952293944</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.5015942791142792</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.6158563234002784</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.7155608086795749</v>
       </c>
     </row>
     <row r="5">
@@ -1123,37 +1286,55 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2866287831520186</v>
+        <v>0.2896103127281016</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1753281944897704</v>
+        <v>0.1642672529150954</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1505645382327084</v>
+        <v>0.144033111131011</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1184258141441213</v>
+        <v>0.1373294827996622</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1172180194014485</v>
+        <v>0.112498823654782</v>
       </c>
       <c r="G5" t="n">
-        <v>0.07666497152403443</v>
+        <v>0.07972325645324015</v>
       </c>
       <c r="H5" t="n">
-        <v>0.07516967905589848</v>
+        <v>0.0725377603181076</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4322642050949457</v>
+        <v>0.3260743075619216</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2524110259847268</v>
+        <v>0.223027783869141</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1656261448010035</v>
+        <v>0.1647762215428352</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1496986241193239</v>
+        <v>0.152878617140578</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1332430698855241</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.3596946139873548</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.1785809463247687</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.162705087356202</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.1596818088693915</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.1393375434622828</v>
       </c>
     </row>
   </sheetData>
@@ -1167,7 +1348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1178,22 +1359,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>F1: 1</t>
+          <t>F2: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>F1: 2</t>
+          <t>F2: 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>F1: 3</t>
+          <t>F2: 3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F1: 4</t>
+          <t>F2: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F2: 5</t>
         </is>
       </c>
     </row>
@@ -1204,16 +1390,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.429027041354204</v>
+        <v>4.890284008387104</v>
       </c>
       <c r="C2" t="n">
-        <v>3.170159058870136</v>
+        <v>2.42792500097139</v>
       </c>
       <c r="D2" t="n">
-        <v>2.08018338849591</v>
+        <v>2.212082293812811</v>
       </c>
       <c r="E2" t="n">
-        <v>1.880141517197375</v>
+        <v>2.170978841433984</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.894385220306634</v>
       </c>
     </row>
     <row r="3">
@@ -1223,16 +1412,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2857382653344318</v>
+        <v>0.2573833688624791</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1668504767826388</v>
+        <v>0.1277855263669153</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1094833362366268</v>
+        <v>0.1164253838848848</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09895481669459867</v>
+        <v>0.1142620442859991</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0997044852792965</v>
       </c>
     </row>
     <row r="4">
@@ -1242,16 +1434,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2857382653344318</v>
+        <v>0.2573833688624791</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4525887421170706</v>
+        <v>0.3851688952293944</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5620720783536974</v>
+        <v>0.5015942791142792</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6610268950482961</v>
+        <v>0.6158563234002784</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.7155608086795749</v>
       </c>
     </row>
     <row r="5">
@@ -1261,16 +1456,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4322642050949457</v>
+        <v>0.3596946139873548</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2524110259847268</v>
+        <v>0.1785809463247687</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1656261448010035</v>
+        <v>0.162705087356202</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1496986241193239</v>
+        <v>0.1596818088693915</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1393375434622828</v>
       </c>
     </row>
   </sheetData>
@@ -1310,12 +1508,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['QSERV', 'PPUNIT', 'QEDLESHI', 'QESL', 'QEXTRCT', 'QHISPC', 'QNOHLTH', 'PERCAP', 'QFHH', 'QRICH', 'QRENTER', 'QPOVTY', 'QNOAUTO', 'QFAM', 'QAGEDEP', 'MEDAGE', 'QSSBEN', 'QFEMLBR', 'QFEMALE']]</t>
+          <t>[['QNOHLTH', 'QHISPC', 'PPUNIT', 'QSERV', 'QESL', 'QEDLESHI', 'QEXTRCT', 'QFHH', 'PERCAP', 'QRICH', 'MDHSEVAL', 'QRENTER', 'QNOAUTO', 'QPOVTY', 'MEDAGE', 'QSSBEN', 'QAGEDEP', 'QFEMLBR', 'QFEMALE']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[['MDGRENT', 'MDHSEVAL', 'QASIAN', 'QBLACK', 'QCVLUN', 'QMOHO', 'QNATIVE', 'QUNOCCHU']]</t>
+          <t>[['MDGRENT', 'QASIAN', 'QBLACK', 'QCVLUN', 'QFAM', 'QMOHO', 'QNATIVE', 'QUNOCCHU']]</t>
         </is>
       </c>
     </row>

</xml_diff>